<commit_message>
revised code and addition of region-specific fitness estimates for 2017 data
</commit_message>
<xml_diff>
--- a/fitness estimates.xlsx
+++ b/fitness estimates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mason Kulbaba\Dropbox\git\geum-aster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49448E65-3BF6-4FB8-9DC1-9B308F1AE63C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5381DF6B-9103-44EA-930A-853D28F2A803}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{E14D7B90-7165-4BC8-AD50-718AF72405F0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Fitness Estimates for 'Regions'</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC05DA3-09FB-4DE4-AB1E-A943DC16B1EC}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,6 +499,48 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2017</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>576.43600000000004</v>
+      </c>
+      <c r="D8">
+        <v>125.247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>93.6</v>
+      </c>
+      <c r="D9">
+        <v>64.409000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2017</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>65.652000000000001</v>
+      </c>
+      <c r="D10">
+        <v>63.234999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Oops! Previous commit did not use sum of 2016 and 2017 seed mass as total fitness for 2017 analysis. This update corrects that, and also provides updated fitness estiamtes to spreadsheet
</commit_message>
<xml_diff>
--- a/fitness estimates.xlsx
+++ b/fitness estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mason Kulbaba\Dropbox\git\geum-aster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5381DF6B-9103-44EA-930A-853D28F2A803}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF30F479-4DA3-4898-B8A0-4B738C1BA78F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{E14D7B90-7165-4BC8-AD50-718AF72405F0}"/>
   </bookViews>
@@ -507,10 +507,10 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>576.43600000000004</v>
+        <v>544.65099999999995</v>
       </c>
       <c r="D8">
-        <v>125.247</v>
+        <v>163.02699999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>93.6</v>
       </c>
       <c r="D9">
-        <v>64.409000000000006</v>
+        <v>81.897999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -535,10 +535,10 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>65.652000000000001</v>
+        <v>70.379000000000005</v>
       </c>
       <c r="D10">
-        <v>63.234999999999999</v>
+        <v>75.872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally fixed 'direction of recession' error in 2018 analysis. Also, completed 2018 analysis to produce region-specific estiamtes of fitness. These fitness estimates have also been included in the spreadsheet.
</commit_message>
<xml_diff>
--- a/fitness estimates.xlsx
+++ b/fitness estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mason Kulbaba\Dropbox\git\geum-aster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF30F479-4DA3-4898-B8A0-4B738C1BA78F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD526A49-0135-4E8F-8484-DC573AA8B971}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{E14D7B90-7165-4BC8-AD50-718AF72405F0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Fitness Estimates for 'Regions'</t>
   </si>
@@ -416,16 +416,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC05DA3-09FB-4DE4-AB1E-A943DC16B1EC}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -499,18 +500,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2017</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>544.65099999999995</v>
+      </c>
+      <c r="D7">
+        <v>163.02699999999999</v>
+      </c>
+    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2017</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>544.65099999999995</v>
+        <v>93.6</v>
       </c>
       <c r="D8">
-        <v>163.02699999999999</v>
+        <v>81.897999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -518,27 +533,55 @@
         <v>2017</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>93.6</v>
+        <v>70.379000000000005</v>
       </c>
       <c r="D9">
-        <v>81.897999999999996</v>
+        <v>75.872</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>926.32399999999996</v>
+      </c>
+      <c r="D10">
+        <v>268.49599999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2018</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>248.6</v>
+      </c>
+      <c r="D11">
+        <v>194.65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2018</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C10">
-        <v>70.379000000000005</v>
-      </c>
-      <c r="D10">
-        <v>75.872</v>
+      <c r="C12">
+        <v>94.444999999999993</v>
+      </c>
+      <c r="D12">
+        <v>100.45399999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>